<commit_message>
Finish basic api backend, update controller, update security, vv....
</commit_message>
<xml_diff>
--- a/REQUIREMENT/EndpointBackend.xlsx
+++ b/REQUIREMENT/EndpointBackend.xlsx
@@ -27,17 +27,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="186">
+  <si>
+    <t>Front-End</t>
+  </si>
+  <si>
+    <t>Back-End</t>
+  </si>
+  <si>
+    <t>Axios</t>
+  </si>
+  <si>
+    <t>Websocket</t>
+  </si>
   <si>
     <t>Endpoint</t>
   </si>
   <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
     <t>Public</t>
   </si>
   <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>String token</t>
+  </si>
+  <si>
     <t>Không cần đăng nhập</t>
   </si>
   <si>
+    <t>POST</t>
+  </si>
+  <si>
     <t>/api/register</t>
   </si>
   <si>
@@ -47,12 +77,48 @@
     <t>AuthController</t>
   </si>
   <si>
+    <t>String userName
+String email
+String password
+String rePassword</t>
+  </si>
+  <si>
+    <t>RegisterRequest</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+String response 
+(Resonse này sẽ trả về text, nếu thành công thì là "Sucessfull" còn thất bại thì sẽ in ra lý do lỗi)</t>
+  </si>
+  <si>
+    <t>RegisterResponse</t>
+  </si>
+  <si>
     <t>/api/login</t>
   </si>
   <si>
     <t>Api đăng nhập tài khoản</t>
   </si>
   <si>
+    <t>String userName
+String password</t>
+  </si>
+  <si>
+    <t>LoginRequest</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+String response 
+(Tương tự phía trên!)
+String token</t>
+  </si>
+  <si>
+    <t>LoginResponse</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
     <t>/api/products</t>
   </si>
   <si>
@@ -62,24 +128,74 @@
     <t>ProductController</t>
   </si>
   <si>
+    <t>Nope</t>
+  </si>
+  <si>
+    <t>Map&lt; String productType, List&lt;ProductResponse&gt;&gt; ProductList</t>
+  </si>
+  <si>
+    <t>ProductListWithTypeResponse</t>
+  </si>
+  <si>
+    <t>PS: ProductResponse: 
+long productId
+String productName
+String productTypeName
+long price
+int discount
+String imageUrl</t>
+  </si>
+  <si>
     <t>/api/product-types</t>
   </si>
   <si>
     <t>Api lấy danh sách loại sản phẩm</t>
   </si>
   <si>
+    <t>List&lt;ProductTypeResponse&gt; ProductTypeList</t>
+  </si>
+  <si>
+    <t>ProductTypeListResponse</t>
+  </si>
+  <si>
+    <t>PS: ProductTypeResponse
+long productTypeId
+String productTypeName</t>
+  </si>
+  <si>
     <t>/api/product?id=</t>
   </si>
   <si>
     <t>Api lấy thông tin chi tiết của sản phẩm</t>
   </si>
   <si>
+    <t>long productId 
+(Id nằm ở đường link luôn)</t>
+  </si>
+  <si>
+    <t>Seller sellerInformation
+String productDescription</t>
+  </si>
+  <si>
+    <t>UserProductDetailResponse</t>
+  </si>
+  <si>
     <t>/api/search</t>
   </si>
   <si>
     <t>Api tìm kiếm sản phẩm</t>
   </si>
   <si>
+    <t>String keyWord 
+(Tương tự thằng trên, keyWord nhận ở đường link luôn)</t>
+  </si>
+  <si>
+    <t>List&lt;ProductResponse&gt; ProductList</t>
+  </si>
+  <si>
+    <t>ProductListResponse</t>
+  </si>
+  <si>
     <t>User</t>
   </si>
   <si>
@@ -92,49 +208,142 @@
     <t>AccountController</t>
   </si>
   <si>
+    <t>String userName
+String email
+Timestamp createdDate</t>
+  </si>
+  <si>
+    <t>AccountResponse</t>
+  </si>
+  <si>
     <t>/api/user/profile</t>
   </si>
   <si>
     <t>Api lấy thông tin profile</t>
   </si>
   <si>
+    <t>String fullName
+String phone
+String address</t>
+  </si>
+  <si>
+    <t>ProfileResponse</t>
+  </si>
+  <si>
     <t>/api/user/update-profile</t>
   </si>
   <si>
     <t>Api thay đổi thông tin cá nhân</t>
   </si>
   <si>
-    <t>/api/user/cart</t>
-  </si>
-  <si>
-    <t>Api lấy thông tin đơn hàng bao gồm sản phẩm có chứa bên trong</t>
+    <t>String fullName
+String phone
+String address 
+(Nếu thông tin trả về của thuộc tính nào = null thì 0 thay đổi!)</t>
+  </si>
+  <si>
+    <t>UpdateProfileRequest</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+(Profile không có giới hạn nên sẽ không sinh ra lỗi)
+String response</t>
+  </si>
+  <si>
+    <t>UpdateProfileResponse</t>
+  </si>
+  <si>
+    <t>/api/user/cart?cartId=?</t>
+  </si>
+  <si>
+    <t>Api lấy thông tin giỏ hàng bao gồm sản phẩm có chứa bên trong 
+(Nếu không có cartId thì lấy giỏ hàng hiện tại, còn không thì lấy theo cartId)</t>
   </si>
   <si>
     <t>CartController</t>
   </si>
   <si>
+    <t>long cartId</t>
+  </si>
+  <si>
+    <t>long cartId
+String phone
+String address
+long totalPrice
+Map&lt;ProductResponse, int quantity&gt; cartItems</t>
+  </si>
+  <si>
+    <t>CartDetailResponse: 
+Lấy thông tin 
+chi tiết của giỏ hàng</t>
+  </si>
+  <si>
     <t>/api/user/add-product?productid=?</t>
   </si>
   <si>
     <t>Api thêm sản phẩm vào giỏ hàng</t>
   </si>
   <si>
+    <t>long productId
+int quantity</t>
+  </si>
+  <si>
+    <t>HandleCartRequest</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+(Ở đây quantity bắt buộc phải lớn hơn 1)
+String response</t>
+  </si>
+  <si>
+    <t>HandleCartResponse</t>
+  </si>
+  <si>
     <t>/api/user/update-product?productid=?</t>
   </si>
   <si>
     <t>Api cập nhật số lượng sản phẩm của 1 sản phẩm cụ thế trong giỏ hàng</t>
   </si>
   <si>
+    <t>Boolean isSuccess
+(Ở đây không có giới hạn quantity nhưng nếu hàng tồn kho hét thì sẽ update không thành công)
+String response</t>
+  </si>
+  <si>
     <t>/api/user/delete-product?productid=?</t>
   </si>
   <si>
     <t>Api xóa sản phẩm ra khỏi giỏ hàng</t>
   </si>
   <si>
+    <t>long productId
+int quantity 
+(Ở đây thì quantity mặc định là 0, có nghĩa là nó sẽ xóa sản phẩm khỏi giỏ hàng)</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+(Ở đây quantity mặc định là 0)
+String response</t>
+  </si>
+  <si>
     <t>/api/user/cart-history</t>
   </si>
   <si>
-    <t>Api lấy thông tin các đơn hàng đã hoàn thành</t>
+    <t>Api lấy thông tin tất cả các giỏ hàng</t>
+  </si>
+  <si>
+    <t>List&lt;CartInfomation&gt; CartHistory</t>
+  </si>
+  <si>
+    <t>CartHistoryResponse</t>
+  </si>
+  <si>
+    <t>PS: CartInformation:
+String cartId
+String phone
+String address
+Timestamp finishedDate
+long totalPrice</t>
   </si>
   <si>
     <t>/api/user/add-feedback?productid=?</t>
@@ -146,46 +355,99 @@
     <t>FeedbackController</t>
   </si>
   <si>
+    <t>long productId
+String feedBack</t>
+  </si>
+  <si>
+    <t>UserHandleFeedBackRequest</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+(Ở đây feedBack bắt buộc phải khác null)
+String response</t>
+  </si>
+  <si>
+    <t>UserHandleFeedBackResponse</t>
+  </si>
+  <si>
     <t>/api/user/update-feedback?productid=?</t>
   </si>
   <si>
     <t>Api cập nhật feedback của 1 sản phẩm</t>
   </si>
   <si>
+    <t>Boolean isSuccess
+String response</t>
+  </si>
+  <si>
     <t>/api/user/delete-feedback?productid=?</t>
   </si>
   <si>
     <t>Api xóa feedback của 1 sản phẩm</t>
   </si>
   <si>
+    <t>long productId
+String feedBack=""</t>
+  </si>
+  <si>
+    <t>Boolean isSuccess
+(Ở đây feedBack mặc định là "")
+String response</t>
+  </si>
+  <si>
     <t>/api/user/feedback-history</t>
   </si>
   <si>
     <t xml:space="preserve">Api lấy thông tin lịch sử comment </t>
   </si>
   <si>
+    <t>Chắc cái này dell cần đâu!</t>
+  </si>
+  <si>
     <t>/api/user/pay-online?cartid=?</t>
   </si>
   <si>
-    <t>Api tạo 1 thanh toán online cho người dùng thanh toán đơn hàng</t>
+    <t>Api tạo 1 thanh toán online cho người dùng thanh toán giỏ hàng</t>
   </si>
   <si>
     <t>PaymentController</t>
   </si>
   <si>
+    <t>PaymentResponse</t>
+  </si>
+  <si>
     <t>/api/user/payment-history?cartid=</t>
   </si>
   <si>
     <t>Api lấy thông tin lịch sử thanh toán dựa theo mã giỏ hàng</t>
   </si>
   <si>
-    <t>/api/user/cancel-order</t>
+    <t>List&lt;PaymentResponse&gt; paymentHistory</t>
+  </si>
+  <si>
+    <t>PaymentHistoryResponse</t>
+  </si>
+  <si>
+    <t>PS: PaymentResponse:
+String paymentId
+String cartId
+long totalPrice
+Timestamp createdDate</t>
+  </si>
+  <si>
+    <t>/api/user/cancel-order?cartId=?</t>
   </si>
   <si>
     <t>Api hủy order và hoàn tiền nếu trả online</t>
   </si>
   <si>
-    <t>/api/user/order</t>
+    <t>OrderController</t>
+  </si>
+  <si>
+    <t>HandleOrderResponse</t>
+  </si>
+  <si>
+    <t>/api/user/order?cartId=?</t>
   </si>
   <si>
     <t>Api tạo order từ giỏ hàng và thay đổi trạng thái đơn hàng</t>
@@ -206,12 +468,43 @@
     <t>Api lấy danh sách sản phẩm của seller</t>
   </si>
   <si>
+    <t>/api/seller/product?productId=?</t>
+  </si>
+  <si>
+    <t>long productId
+int quantity
+boolean isActive
+Timestamp postedDate
+int sale
+String productDescription</t>
+  </si>
+  <si>
+    <t>SellerProductDetailResponse</t>
+  </si>
+  <si>
     <t>/api/seller/add-product</t>
   </si>
   <si>
     <t>Api thêm sản phẩm mới</t>
   </si>
   <si>
+    <t>long productId
+String productName
+String productTypeName
+int quantity
+boolean isActive
+int discount
+long price
+String description
+String imageUrl</t>
+  </si>
+  <si>
+    <t>HandleProductRequest</t>
+  </si>
+  <si>
+    <t>HandleProductResponse</t>
+  </si>
+  <si>
     <t>/api/seller/update-product</t>
   </si>
   <si>
@@ -227,19 +520,51 @@
     <t>Api lấy danh sách đơn hàng hiện có</t>
   </si>
   <si>
+    <t>List&lt;OrderResponse&gt; OrderListResponse</t>
+  </si>
+  <si>
+    <t>OrderListResponse</t>
+  </si>
+  <si>
+    <t>PS: OrderResponse:
+long orderId
+long cartId
+long productId
+int quantity
+OrderStatus status
+(Ở đây status chỉ lấy "ORDERED")</t>
+  </si>
+  <si>
     <t>/api/seller/order-history</t>
   </si>
   <si>
     <t>Api xem lịch sử đơn hàng</t>
   </si>
   <si>
-    <t>/api/seller/accept-order</t>
+    <t>List&lt;OrderResponse&gt; OrderHistoryResponse</t>
+  </si>
+  <si>
+    <t>OrderHistoryResponse</t>
+  </si>
+  <si>
+    <t>PS: OrderResponse:
+long orderId
+long cartId
+long productId
+int quantity
+OrderStatus status</t>
+  </si>
+  <si>
+    <t>/api/seller/accept-order?orderId=?</t>
   </si>
   <si>
     <t>Api xác thực seller chấp nhận đơn hàng</t>
   </si>
   <si>
-    <t>/api/seller/cancel-order</t>
+    <t>long orderId</t>
+  </si>
+  <si>
+    <t>/api/seller/cancel-order?orderId=?</t>
   </si>
   <si>
     <t>Api hủy đơn hàng</t>
@@ -248,18 +573,58 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>/api/admin/accounts</t>
+    <t>/api/admin/role</t>
+  </si>
+  <si>
+    <t>Api lấy danh sách role</t>
+  </si>
+  <si>
+    <t>List&lt;Role&gt; RoleResponse</t>
+  </si>
+  <si>
+    <t>RoleListResponse</t>
+  </si>
+  <si>
+    <t>/api/admin/accounts?role=?</t>
   </si>
   <si>
     <t>Api lấy danh sách tất cả tài khoản, chia theo role</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Map&lt;Role, List&lt;AccountResponse&gt;&gt; AccountListResponse</t>
+  </si>
+  <si>
+    <t>AccountListWithRoleResponse</t>
+  </si>
+  <si>
+    <t>PS: AccountResponse:
+String userName
+String email
+Timestamp createdDate</t>
+  </si>
+  <si>
     <t>/api/admin/update-account</t>
   </si>
   <si>
     <t>Api cập nhật thông tin tài khoản của role nhỏ hơn admin</t>
   </si>
   <si>
+    <t>String userName
+String email
+String password
+Role role
+boolean isActive</t>
+  </si>
+  <si>
+    <t>UpdateAccountRequest</t>
+  </si>
+  <si>
+    <t>UpdateAccountResponse</t>
+  </si>
+  <si>
     <t>/api/admin/products</t>
   </si>
   <si>
@@ -278,28 +643,36 @@
     <t>Api xóa sản phẩm (thay đổi thành unavailable)</t>
   </si>
   <si>
-    <t>/api/admin/orders</t>
-  </si>
-  <si>
-    <t>Api lấy danh sách các đơn hàng hiện tại</t>
-  </si>
-  <si>
-    <t>/api/admin/order-history</t>
-  </si>
-  <si>
-    <t>Api lấy danh sách các đơn hàng đã hoàn thành</t>
-  </si>
-  <si>
-    <t>/api/admin/payments</t>
-  </si>
-  <si>
-    <t>Api lấy danh sách các khoản thanh toán nhưng đơn hàng chưa hoàn thành</t>
+    <t>/api/admin/cart?cartId=?</t>
+  </si>
+  <si>
+    <t>Api lấy thông tin chi tiết đơn hàng của người dùng</t>
+  </si>
+  <si>
+    <t>PS: ProductResponse: 
+long productId
+String productName
+long price
+int discount
+String imageUrl</t>
+  </si>
+  <si>
+    <t>/api/admin/cart-history</t>
+  </si>
+  <si>
+    <t>Api lấy danh sách các đơn hàng</t>
+  </si>
+  <si>
+    <t>/api/admin/payments?paymentId=?</t>
+  </si>
+  <si>
+    <t>Api lấy thông tin chi tiết thanh toán</t>
   </si>
   <si>
     <t>/api/admin/payment-history</t>
   </si>
   <si>
-    <t>Api lấy danh sách các khoản thanh toán của đơn hàng đã hoàn thành</t>
+    <t>Api lấy danh sách các khoản thanh toán</t>
   </si>
   <si>
     <t>/api/admin/feedbacks</t>
@@ -321,10 +694,31 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -474,7 +868,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="53">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,12 +877,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF018D2C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF475FF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -519,7 +931,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7E719F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5655E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBD3A3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9AC6A3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A6B98"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD98D59"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95A3C6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -830,97 +1308,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -929,53 +1362,107 @@
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -986,6 +1473,99 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1255,6 +1835,20 @@
       <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="00475FF6"/>
+      <color rgb="007E719F"/>
+      <color rgb="00B5655E"/>
+      <color rgb="009AC6A3"/>
+      <color rgb="004A6B98"/>
+      <color rgb="00D98D59"/>
+      <color rgb="007B6993"/>
+      <color rgb="0095A3C6"/>
+      <color rgb="00863E56"/>
+      <color rgb="00EBD3A3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1521,543 +2115,1346 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.6952380952381" customWidth="1"/>
-    <col min="3" max="3" width="33.7619047619048" customWidth="1"/>
-    <col min="4" max="4" width="64.8095238095238" customWidth="1"/>
-    <col min="5" max="5" width="20.7714285714286" customWidth="1"/>
+    <col min="3" max="3" width="7.14285714285714" customWidth="1"/>
+    <col min="4" max="4" width="33.7619047619048" customWidth="1"/>
+    <col min="5" max="5" width="64.8095238095238" customWidth="1"/>
+    <col min="6" max="6" width="20.7714285714286" customWidth="1"/>
+    <col min="7" max="7" width="25.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="25.8095238095238" customWidth="1"/>
+    <col min="9" max="9" width="14.3904761904762" customWidth="1"/>
+    <col min="10" max="11" width="13.6190476190476" customWidth="1"/>
+    <col min="12" max="12" width="14.2761904761905" customWidth="1"/>
+    <col min="13" max="13" width="39.3333333333333" customWidth="1"/>
+    <col min="14" max="14" width="27.1333333333333" customWidth="1"/>
+    <col min="15" max="15" width="22.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="7:14">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="1" t="s">
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="7:14">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="1"/>
-      <c r="C5" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
+      <c r="N4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="75" spans="1:14">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" ht="60" spans="1:14">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" ht="105" spans="1:15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" ht="60" spans="1:15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" ht="30" spans="1:14">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" ht="105" spans="1:15">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" ht="45" spans="1:14">
+      <c r="A12" s="3"/>
+      <c r="C12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" ht="45" spans="1:14">
+      <c r="A13" s="3"/>
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" ht="90" spans="1:14">
+      <c r="A14" s="3"/>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" ht="105" spans="1:15">
+      <c r="A15" s="3"/>
+      <c r="C15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" ht="45" spans="1:14">
+      <c r="A16" s="3"/>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="1:14">
+      <c r="A17" s="3"/>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" ht="75" spans="1:14">
+      <c r="A18" s="3"/>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" ht="90" spans="1:15">
+      <c r="A19" s="3"/>
+      <c r="C19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="O19" s="36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" ht="45" spans="3:14">
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="N20" s="38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" ht="30" spans="3:14">
+      <c r="C21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="N21" s="38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" ht="45" spans="3:14">
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+    </row>
+    <row r="24" ht="30" spans="3:14">
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="N24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" ht="75" spans="3:15">
+      <c r="C25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" t="s">
+        <v>112</v>
+      </c>
+      <c r="N25" t="s">
+        <v>113</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" ht="30" spans="3:14">
+      <c r="C26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="N26" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" ht="30" spans="3:14">
+      <c r="C27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="N27" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" ht="45" spans="1:14">
+      <c r="A29" s="3"/>
+      <c r="C29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" ht="45" spans="1:14">
+      <c r="A30" s="3"/>
+      <c r="C30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" ht="90" spans="1:14">
+      <c r="A31" s="3"/>
+      <c r="C31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="N31" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" ht="105" spans="1:15">
+      <c r="A32" s="3"/>
+      <c r="C32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" ht="90" spans="1:14">
+      <c r="A33" s="3"/>
+      <c r="C33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" ht="135" spans="1:14">
+      <c r="A34" s="3"/>
+      <c r="C34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" t="s">
+        <v>132</v>
+      </c>
+      <c r="M34" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="N34" s="42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" ht="135" spans="1:14">
+      <c r="A35" s="3"/>
+      <c r="C35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35" t="s">
+        <v>132</v>
+      </c>
+      <c r="M35" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="N35" s="42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" ht="135" spans="1:14">
+      <c r="A36" s="3"/>
+      <c r="C36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36" t="s">
+        <v>132</v>
+      </c>
+      <c r="M36" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="N36" s="42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" ht="120" spans="3:15">
+      <c r="C37" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+      <c r="M37" t="s">
+        <v>139</v>
+      </c>
+      <c r="N37" t="s">
+        <v>140</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" ht="90" spans="3:15">
+      <c r="C38" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" t="s">
+        <v>30</v>
+      </c>
+      <c r="M38" t="s">
+        <v>144</v>
+      </c>
+      <c r="N38" t="s">
+        <v>145</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" ht="30" spans="3:14">
+      <c r="C39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" t="s">
+        <v>30</v>
+      </c>
+      <c r="M39" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="N39" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" ht="30" spans="3:14">
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" t="s">
+        <v>149</v>
+      </c>
+      <c r="H40" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="N40" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14">
+      <c r="C42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+      <c r="M42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" ht="60" spans="1:15">
+      <c r="A43" s="3"/>
+      <c r="C43" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" t="s">
+        <v>160</v>
+      </c>
+      <c r="N43" t="s">
+        <v>161</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" ht="75" spans="1:14">
+      <c r="A44" s="3"/>
+      <c r="C44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H44" t="s">
+        <v>166</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="N44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" ht="105" spans="1:15">
+      <c r="A45" s="3"/>
+      <c r="C45" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" t="s">
+        <v>30</v>
+      </c>
+      <c r="M45" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N45" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="O45" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="4"/>
+      <c r="C47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" ht="90" spans="1:15">
+      <c r="A48" s="3"/>
+      <c r="C48" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" t="s">
+        <v>175</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" t="s">
+        <v>30</v>
+      </c>
+      <c r="M48" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="N48" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="O48" s="32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" ht="90" spans="3:15">
+      <c r="C49" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" t="s">
+        <v>178</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" t="s">
+        <v>30</v>
+      </c>
+      <c r="M49" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="N49" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="O49" s="36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>179</v>
+      </c>
+      <c r="E50" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6">
+      <c r="C51" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>181</v>
+      </c>
+      <c r="E51" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6">
+      <c r="C52" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" t="s">
+        <v>184</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="3"/>
+      <c r="C54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5">
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5">
-      <c r="C11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5">
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5">
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5">
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5">
-      <c r="C15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5">
-      <c r="C16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5">
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5">
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5">
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5">
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5">
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5">
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5">
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5">
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5">
-      <c r="C27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5">
-      <c r="C28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5">
-      <c r="C29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5">
-      <c r="C30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5">
-      <c r="C31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5">
-      <c r="C32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5">
-      <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5">
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5">
-      <c r="C36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5">
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5">
-      <c r="C39" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5">
-      <c r="C40" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5">
-      <c r="C41" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="1"/>
-      <c r="C43" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5">
-      <c r="C44" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" t="s">
-        <v>84</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5">
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5">
-      <c r="C46" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5">
-      <c r="C47" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5">
-      <c r="C48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5">
-      <c r="C50" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2" t="s">
-        <v>5</v>
+      <c r="H54" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B42:B43"/>
+  <mergeCells count="13">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="G23:N23"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>